<commit_message>
Upload new alternative evaluation via file upload
</commit_message>
<xml_diff>
--- a/alternative_eval/Alternatives Matrix.xlsx
+++ b/alternative_eval/Alternatives Matrix.xlsx
@@ -351,11 +351,11 @@
         <v>-20</v>
       </c>
       <c r="H3" s="11">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="I3" s="12" t="str">
         <f t="shared" ref="I3:I7" si="5">B3*H3</f>
-        <v>-25</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="4" ht="26.25" customHeight="1">
@@ -402,11 +402,11 @@
         <v>13</v>
       </c>
       <c r="D5" s="7">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E5" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>-8</v>
+        <v>-12</v>
       </c>
       <c r="F5" s="9">
         <v>3.0</v>
@@ -495,7 +495,7 @@
       <c r="A8" s="13"/>
       <c r="E8" s="15" t="str">
         <f>sum(E3:E7)</f>
-        <v>-5</v>
+        <v>-9</v>
       </c>
       <c r="G8" s="16" t="str">
         <f>sum(G3:G7)</f>
@@ -504,7 +504,7 @@
       <c r="H8" s="17"/>
       <c r="I8" s="18" t="str">
         <f>sum(I3:I7)</f>
-        <v>-31</v>
+        <v>-21</v>
       </c>
       <c r="T8" s="14"/>
     </row>

</xml_diff>